<commit_message>
he terminado de añadir todas las zonas y he corregido la pasarela para SIOSE, ya que habia algunos codigos que no coincidian
</commit_message>
<xml_diff>
--- a/Correspondencias_SIOSE - modificada (v4).xlsx
+++ b/Correspondencias_SIOSE - modificada (v4).xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="276" uniqueCount="164">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="278" uniqueCount="165">
   <si>
     <t>SIOSE</t>
   </si>
@@ -465,9 +465,6 @@
     <t>Pastizal arbolado: coniferas. disperso</t>
   </si>
   <si>
-    <t>SIN ASIGNACIoN</t>
-  </si>
-  <si>
     <t>Via de comunicacion no asfaltada</t>
   </si>
   <si>
@@ -529,6 +526,12 @@
   </si>
   <si>
     <t>CULTIVOS HERBACEOS Y LEÑOSOS EN SECANO</t>
+  </si>
+  <si>
+    <t>SIN ASIGNACION</t>
+  </si>
+  <si>
+    <t>CULTIVOS HERBACEOS Y LEÃ‘OSOS REGADOS</t>
   </si>
 </sst>
 </file>
@@ -754,7 +757,7 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="25">
+  <cellXfs count="26">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="2" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="2" applyFont="1"/>
@@ -806,6 +809,7 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2" applyFont="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="40% - Énfasis5" xfId="1" builtinId="47"/>
@@ -1088,10 +1092,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F89"/>
+  <dimension ref="A1:F91"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A49" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="F90" sqref="F90"/>
+    <sheetView tabSelected="1" topLeftCell="A43" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="D91" sqref="C87:D91"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1125,8 +1129,8 @@
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A2" s="6" t="s">
-        <v>142</v>
+      <c r="A2" s="25" t="s">
+        <v>163</v>
       </c>
       <c r="B2" s="7">
         <v>0</v>
@@ -1435,7 +1439,7 @@
         <v>131</v>
       </c>
       <c r="D17" s="8" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="E17" s="9">
         <v>4</v>
@@ -1455,7 +1459,7 @@
         <v>131</v>
       </c>
       <c r="D18" s="8" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="E18" s="9">
         <v>4</v>
@@ -1475,13 +1479,13 @@
         <v>141</v>
       </c>
       <c r="D19" s="8" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="E19" s="9">
         <v>5</v>
       </c>
       <c r="F19" s="10" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.25">
@@ -1695,7 +1699,7 @@
         <v>193</v>
       </c>
       <c r="D30" s="8" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="E30" s="9">
         <v>11</v>
@@ -1795,7 +1799,7 @@
         <v>211</v>
       </c>
       <c r="D35" s="8" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="E35" s="9">
         <v>12</v>
@@ -1815,7 +1819,7 @@
         <v>217</v>
       </c>
       <c r="D36" s="8" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="E36" s="9">
         <v>12</v>
@@ -1835,7 +1839,7 @@
         <v>215</v>
       </c>
       <c r="D37" s="8" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="E37" s="9">
         <v>12</v>
@@ -1855,7 +1859,7 @@
         <v>217</v>
       </c>
       <c r="D38" s="8" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="E38" s="9">
         <v>12</v>
@@ -1955,7 +1959,7 @@
         <v>44</v>
       </c>
       <c r="D43" s="8" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="E43" s="9">
         <v>16</v>
@@ -1995,13 +1999,13 @@
         <v>331</v>
       </c>
       <c r="D45" s="8" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="E45" s="9">
         <v>17</v>
       </c>
       <c r="F45" s="10" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
     </row>
     <row r="46" spans="1:6" x14ac:dyDescent="0.25">
@@ -2021,7 +2025,7 @@
         <v>17</v>
       </c>
       <c r="F46" s="10" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
     </row>
     <row r="47" spans="1:6" x14ac:dyDescent="0.25">
@@ -2041,7 +2045,7 @@
         <v>17</v>
       </c>
       <c r="F47" s="10" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
     </row>
     <row r="48" spans="1:6" x14ac:dyDescent="0.25">
@@ -2315,7 +2319,7 @@
         <v>520</v>
       </c>
       <c r="D61" s="8" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="E61" s="9">
         <v>29</v>
@@ -2335,7 +2339,7 @@
         <v>530</v>
       </c>
       <c r="D62" s="8" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="E62" s="9">
         <v>29</v>
@@ -2775,18 +2779,18 @@
         <v>155</v>
       </c>
       <c r="D84" s="22" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="E84" s="17">
         <v>36</v>
       </c>
       <c r="F84" s="14" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
     </row>
     <row r="85" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A85" s="18" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="B85" s="19" t="s">
         <v>44</v>
@@ -2795,7 +2799,7 @@
         <v>225</v>
       </c>
       <c r="D85" s="18" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="E85" s="17">
         <v>20</v>
@@ -2806,7 +2810,7 @@
     </row>
     <row r="86" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A86" s="21" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="B86" s="19" t="s">
         <v>44</v>
@@ -2815,64 +2819,80 @@
         <v>411</v>
       </c>
       <c r="D86" s="21" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="E86" s="17">
         <v>24</v>
       </c>
       <c r="F86" s="14" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
     </row>
     <row r="87" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A87" s="15" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="C87" s="13">
         <v>425</v>
       </c>
       <c r="D87" s="15" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="E87" s="17">
         <v>25</v>
       </c>
       <c r="F87" s="14" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
     </row>
     <row r="88" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="C88" s="23">
         <v>427</v>
       </c>
       <c r="D88" s="24" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="E88" s="17">
         <v>25</v>
       </c>
       <c r="F88" s="14" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
     </row>
     <row r="89" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="C89" s="23">
         <v>441</v>
       </c>
       <c r="D89" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="E89" s="17">
         <v>27</v>
       </c>
       <c r="F89" s="14" t="s">
         <v>66</v>
+      </c>
+    </row>
+    <row r="90" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="C90" s="23">
+        <v>231</v>
+      </c>
+      <c r="D90" s="18" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="91" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="C91" s="23">
+        <v>451</v>
+      </c>
+      <c r="D91" t="s">
+        <v>164</v>
       </c>
     </row>
   </sheetData>

</xml_diff>